<commit_message>
Changes for Code Coverage
Changes for Code Coverage
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7620" firstSheet="5" activeTab="7"/>
+    <workbookView windowWidth="20490" windowHeight="7620" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="createTimesheet@Admin" sheetId="18" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="95">
   <si>
     <t>Project</t>
   </si>
@@ -242,33 +242,48 @@
     <t>Regional Holiday</t>
   </si>
   <si>
+    <t>Self Learning</t>
+  </si>
+  <si>
+    <t>Task20</t>
+  </si>
+  <si>
+    <t>Analysis(Grooming)</t>
+  </si>
+  <si>
+    <t>Task21</t>
+  </si>
+  <si>
+    <t>Manual Test Case Creation/Updation</t>
+  </si>
+  <si>
+    <t>Task25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automation </t>
+  </si>
+  <si>
+    <t>Task26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QA Review </t>
+  </si>
+  <si>
+    <t>Task28</t>
+  </si>
+  <si>
+    <t>Automation Test Case Execution</t>
+  </si>
+  <si>
     <t>PL</t>
   </si>
   <si>
     <t>SL</t>
   </si>
   <si>
-    <t>BL</t>
-  </si>
-  <si>
-    <t>PAT</t>
-  </si>
-  <si>
     <t>LOP</t>
   </si>
   <si>
-    <t>Task20</t>
-  </si>
-  <si>
-    <t>Analysis(Grooming)</t>
-  </si>
-  <si>
-    <t>Task21</t>
-  </si>
-  <si>
-    <t>Manual Test Case Creation/Updation</t>
-  </si>
-  <si>
     <t>Task22</t>
   </si>
   <si>
@@ -285,9 +300,6 @@
   </si>
   <si>
     <t>Bug Management</t>
-  </si>
-  <si>
-    <t>Task25</t>
   </si>
   <si>
     <r>
@@ -310,9 +322,6 @@
     </r>
   </si>
   <si>
-    <t>Task26</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="9"/>
@@ -337,12 +346,6 @@
   </si>
   <si>
     <t>Automation Test Case Creation/Updation</t>
-  </si>
-  <si>
-    <t>Task28</t>
-  </si>
-  <si>
-    <t>Automation Test Case Execution</t>
   </si>
   <si>
     <t>Task29</t>
@@ -1821,7 +1824,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>13</v>
@@ -1891,7 +1894,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>13</v>
@@ -1982,7 +1985,7 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -2052,7 +2055,7 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
@@ -4636,10 +4639,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:K30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.12380952380952" defaultRowHeight="15"/>
@@ -4723,25 +4726,25 @@
         <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E3" s="3">
         <v>0</v>
       </c>
       <c r="F3" s="3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
       </c>
       <c r="H3" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I3" s="3">
         <v>0</v>
@@ -4758,25 +4761,25 @@
         <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="E4" s="3">
         <v>0</v>
       </c>
       <c r="F4" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
       </c>
       <c r="H4" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I4" s="3">
         <v>0</v>
@@ -4793,25 +4796,25 @@
         <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="E5" s="3">
         <v>0</v>
       </c>
       <c r="F5" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" s="3">
         <v>0</v>
       </c>
       <c r="H5" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="3">
         <v>0</v>
@@ -4828,13 +4831,13 @@
         <v>11</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="E6" s="3">
         <v>0</v>
@@ -4843,10 +4846,10 @@
         <v>0</v>
       </c>
       <c r="G6" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I6" s="3">
         <v>0</v>
@@ -4863,13 +4866,13 @@
         <v>11</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="E7" s="3">
         <v>0</v>
@@ -4878,7 +4881,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H7" s="3">
         <v>0</v>
@@ -4887,7 +4890,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K7" s="3">
         <v>0</v>
@@ -4898,13 +4901,13 @@
         <v>11</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="E8" s="3">
         <v>0</v>
@@ -4913,7 +4916,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H8" s="3">
         <v>0</v>
@@ -4922,7 +4925,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K8" s="3">
         <v>0</v>
@@ -4933,13 +4936,13 @@
         <v>11</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="E9" s="3">
         <v>0</v>
@@ -4948,16 +4951,16 @@
         <v>0</v>
       </c>
       <c r="G9" s="3">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3">
         <v>2</v>
-      </c>
-      <c r="H9" s="3">
-        <v>0</v>
-      </c>
-      <c r="I9" s="3">
-        <v>0</v>
-      </c>
-      <c r="J9" s="3">
-        <v>0</v>
       </c>
       <c r="K9" s="3">
         <v>0</v>
@@ -4968,13 +4971,13 @@
         <v>11</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="E10" s="3">
         <v>0</v>
@@ -4986,13 +4989,13 @@
         <v>0</v>
       </c>
       <c r="H10" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I10" s="3">
         <v>0</v>
       </c>
       <c r="J10" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10" s="3">
         <v>0</v>
@@ -5003,13 +5006,13 @@
         <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>32</v>
+        <v>68</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>69</v>
       </c>
       <c r="E11" s="3">
         <v>0</v>
@@ -5021,7 +5024,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I11" s="3">
         <v>0</v>
@@ -5033,18 +5036,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" ht="16" customHeight="1" spans="1:11">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>53</v>
+        <v>70</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="E12" s="3">
         <v>0</v>
@@ -5056,10 +5059,10 @@
         <v>0</v>
       </c>
       <c r="H12" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I12" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J12" s="3">
         <v>0</v>
@@ -5073,13 +5076,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>67</v>
+        <v>72</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="E13" s="3">
         <v>0</v>
@@ -5091,13 +5094,13 @@
         <v>0</v>
       </c>
       <c r="H13" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I13" s="3">
         <v>0</v>
       </c>
       <c r="J13" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K13" s="3">
         <v>0</v>
@@ -5108,13 +5111,13 @@
         <v>11</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>68</v>
+        <v>74</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="E14" s="3">
         <v>0</v>
@@ -5129,10 +5132,10 @@
         <v>0</v>
       </c>
       <c r="I14" s="3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J14" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K14" s="3">
         <v>0</v>
@@ -5143,13 +5146,13 @@
         <v>11</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>69</v>
+        <v>76</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>77</v>
       </c>
       <c r="E15" s="3">
         <v>0</v>
@@ -5164,537 +5167,12 @@
         <v>0</v>
       </c>
       <c r="I15" s="3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J15" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K15" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E16" s="3">
-        <v>0</v>
-      </c>
-      <c r="F16" s="3">
-        <v>0</v>
-      </c>
-      <c r="G16" s="3">
-        <v>0</v>
-      </c>
-      <c r="H16" s="3">
-        <v>0</v>
-      </c>
-      <c r="I16" s="3">
-        <v>1</v>
-      </c>
-      <c r="J16" s="3">
-        <v>0</v>
-      </c>
-      <c r="K16" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
-      <c r="A17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E17" s="3">
-        <v>0</v>
-      </c>
-      <c r="F17" s="3">
-        <v>0</v>
-      </c>
-      <c r="G17" s="3">
-        <v>0</v>
-      </c>
-      <c r="H17" s="3">
-        <v>0</v>
-      </c>
-      <c r="I17" s="3">
-        <v>0</v>
-      </c>
-      <c r="J17" s="3">
-        <v>2</v>
-      </c>
-      <c r="K17" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
-      <c r="A18" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E18" s="3">
-        <v>0</v>
-      </c>
-      <c r="F18" s="3">
-        <v>0</v>
-      </c>
-      <c r="G18" s="3">
-        <v>0</v>
-      </c>
-      <c r="H18" s="3">
-        <v>0</v>
-      </c>
-      <c r="I18" s="3">
-        <v>0</v>
-      </c>
-      <c r="J18" s="3">
-        <v>4</v>
-      </c>
-      <c r="K18" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
-      <c r="A19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E19" s="3">
-        <v>0</v>
-      </c>
-      <c r="F19" s="3">
-        <v>0</v>
-      </c>
-      <c r="G19" s="3">
-        <v>0</v>
-      </c>
-      <c r="H19" s="3">
-        <v>0</v>
-      </c>
-      <c r="I19" s="3">
-        <v>0</v>
-      </c>
-      <c r="J19" s="3">
-        <v>2</v>
-      </c>
-      <c r="K19" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="A20" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E20" s="3">
-        <v>0</v>
-      </c>
-      <c r="F20" s="3">
-        <v>0</v>
-      </c>
-      <c r="G20" s="3">
-        <v>0</v>
-      </c>
-      <c r="H20" s="3">
-        <v>0</v>
-      </c>
-      <c r="I20" s="3">
-        <v>0</v>
-      </c>
-      <c r="J20" s="3">
-        <v>1</v>
-      </c>
-      <c r="K20" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E21" s="3">
-        <v>0</v>
-      </c>
-      <c r="F21" s="3">
-        <v>0</v>
-      </c>
-      <c r="G21" s="3">
-        <v>0</v>
-      </c>
-      <c r="H21" s="3">
-        <v>2</v>
-      </c>
-      <c r="I21" s="3">
-        <v>0</v>
-      </c>
-      <c r="J21" s="3">
-        <v>0</v>
-      </c>
-      <c r="K21" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="E22" s="3">
-        <v>0</v>
-      </c>
-      <c r="F22" s="3">
-        <v>0</v>
-      </c>
-      <c r="G22" s="3">
-        <v>0</v>
-      </c>
-      <c r="H22" s="3">
-        <v>0</v>
-      </c>
-      <c r="I22" s="3">
-        <v>4</v>
-      </c>
-      <c r="J22" s="3">
-        <v>0</v>
-      </c>
-      <c r="K22" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
-      <c r="A23" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E23" s="3">
-        <v>0</v>
-      </c>
-      <c r="F23" s="3">
-        <v>0</v>
-      </c>
-      <c r="G23" s="3">
-        <v>0</v>
-      </c>
-      <c r="H23" s="3">
-        <v>0</v>
-      </c>
-      <c r="I23" s="3">
-        <v>4</v>
-      </c>
-      <c r="J23" s="3">
-        <v>0</v>
-      </c>
-      <c r="K23" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
-      <c r="A24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E24" s="3">
-        <v>0</v>
-      </c>
-      <c r="F24" s="3">
-        <v>0</v>
-      </c>
-      <c r="G24" s="3">
-        <v>0</v>
-      </c>
-      <c r="H24" s="3">
-        <v>0</v>
-      </c>
-      <c r="I24" s="3">
-        <v>1</v>
-      </c>
-      <c r="J24" s="3">
-        <v>0</v>
-      </c>
-      <c r="K24" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
-      <c r="A25" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E25" s="3">
-        <v>0</v>
-      </c>
-      <c r="F25" s="3">
-        <v>0</v>
-      </c>
-      <c r="G25" s="3">
-        <v>0</v>
-      </c>
-      <c r="H25" s="3">
-        <v>0</v>
-      </c>
-      <c r="I25" s="3">
-        <v>0</v>
-      </c>
-      <c r="J25" s="3">
-        <v>2</v>
-      </c>
-      <c r="K25" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11">
-      <c r="A26" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="E26" s="3">
-        <v>0</v>
-      </c>
-      <c r="F26" s="3">
-        <v>0</v>
-      </c>
-      <c r="G26" s="3">
-        <v>0</v>
-      </c>
-      <c r="H26" s="3">
-        <v>0</v>
-      </c>
-      <c r="I26" s="3">
-        <v>0</v>
-      </c>
-      <c r="J26" s="3">
-        <v>4</v>
-      </c>
-      <c r="K26" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
-      <c r="A27" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E27" s="3">
-        <v>0</v>
-      </c>
-      <c r="F27" s="3">
-        <v>0</v>
-      </c>
-      <c r="G27" s="3">
-        <v>0</v>
-      </c>
-      <c r="H27" s="3">
-        <v>0</v>
-      </c>
-      <c r="I27" s="3">
-        <v>0</v>
-      </c>
-      <c r="J27" s="3">
-        <v>2</v>
-      </c>
-      <c r="K27" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11">
-      <c r="A28" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E28" s="3">
-        <v>0</v>
-      </c>
-      <c r="F28" s="3">
-        <v>0</v>
-      </c>
-      <c r="G28" s="3">
-        <v>0</v>
-      </c>
-      <c r="H28" s="3">
-        <v>0</v>
-      </c>
-      <c r="I28" s="3">
-        <v>0</v>
-      </c>
-      <c r="J28" s="3">
-        <v>1</v>
-      </c>
-      <c r="K28" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11">
-      <c r="A29" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E29" s="3">
-        <v>0</v>
-      </c>
-      <c r="F29" s="3">
-        <v>0</v>
-      </c>
-      <c r="G29" s="3">
-        <v>0</v>
-      </c>
-      <c r="H29" s="3">
-        <v>0</v>
-      </c>
-      <c r="I29" s="3">
-        <v>0</v>
-      </c>
-      <c r="J29" s="3">
-        <v>2</v>
-      </c>
-      <c r="K29" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11">
-      <c r="A30" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E30" s="3">
-        <v>0</v>
-      </c>
-      <c r="F30" s="3">
-        <v>0</v>
-      </c>
-      <c r="G30" s="3">
-        <v>0</v>
-      </c>
-      <c r="H30" s="3">
-        <v>0</v>
-      </c>
-      <c r="I30" s="3">
-        <v>0</v>
-      </c>
-      <c r="J30" s="3">
-        <v>1</v>
-      </c>
-      <c r="K30" s="3">
         <v>0</v>
       </c>
     </row>
@@ -5709,7 +5187,7 @@
   <sheetPr/>
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -6151,7 +5629,7 @@
         <v>55</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="E13" s="3">
         <v>0</v>
@@ -6186,7 +5664,7 @@
         <v>55</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="E14" s="3">
         <v>0</v>
@@ -6221,7 +5699,7 @@
         <v>55</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="E15" s="3">
         <v>0</v>
@@ -6256,7 +5734,7 @@
         <v>55</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="E16" s="3">
         <v>0</v>
@@ -6291,7 +5769,7 @@
         <v>55</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E17" s="3">
         <v>0</v>
@@ -6425,13 +5903,13 @@
         <v>11</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E21" s="3">
         <v>0</v>
@@ -6460,13 +5938,13 @@
         <v>11</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E22" s="3">
         <v>0</v>
@@ -6495,13 +5973,13 @@
         <v>11</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="E23" s="3">
         <v>0</v>
@@ -6530,13 +6008,13 @@
         <v>11</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E24" s="3">
         <v>0</v>
@@ -6565,13 +6043,13 @@
         <v>11</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="E25" s="3">
         <v>0</v>
@@ -6600,13 +6078,13 @@
         <v>11</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E26" s="3">
         <v>0</v>
@@ -6635,13 +6113,13 @@
         <v>11</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E27" s="3">
         <v>0</v>
@@ -6670,13 +6148,13 @@
         <v>11</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E28" s="3">
         <v>0</v>
@@ -6705,13 +6183,13 @@
         <v>11</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="E29" s="3">
         <v>0</v>
@@ -6740,13 +6218,13 @@
         <v>11</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E30" s="3">
         <v>0</v>
@@ -6827,7 +6305,7 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -6862,7 +6340,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -6897,7 +6375,7 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>

</xml_diff>